<commit_message>
update results summary file
</commit_message>
<xml_diff>
--- a/code/results/initial_results_testing_ns.xlsx
+++ b/code/results/initial_results_testing_ns.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823FCAFC-F27E-4160-9575-B224C4D9F382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0685F1-A6D8-4DD5-957F-8C61F9DC9621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CEC HW Main Meter Power" sheetId="1" r:id="rId1"/>
+    <sheet name="CEC HW Main Meter Flow" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,9 +30,6 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>CEC_compiled_data_1a_updated.csv</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   <si>
     <t>Identifies a lot of anomalies but also misses a lot, not doing well when data drops, but appears to do generally well with jumps.
 - does this</t>
+  </si>
+  <si>
+    <t>CEC_compiled_data_3a_updated.csv</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,39 +429,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -476,21 +476,21 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>0.15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>60</v>
@@ -505,21 +505,21 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>0.15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>720</v>
@@ -534,16 +534,16 @@
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>